<commit_message>
Added Formula in both read and write
</commit_message>
<xml_diff>
--- a/employee.xlsx
+++ b/employee.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Employee id</t>
   </si>
@@ -21,6 +21,9 @@
   </si>
   <si>
     <t>Department</t>
+  </si>
+  <si>
+    <t>Salary($/month)</t>
   </si>
   <si>
     <t>Aditya</t>
@@ -45,6 +48,9 @@
   </si>
   <si>
     <t>Clerk</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -89,7 +95,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -105,16 +111,22 @@
       <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
         <v>1.0</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>500.0</v>
       </c>
     </row>
     <row r="3">
@@ -122,10 +134,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>300.0</v>
       </c>
     </row>
     <row r="4">
@@ -133,10 +148,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>400.0</v>
       </c>
     </row>
     <row r="5">
@@ -144,10 +162,21 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D6" s="0">
+        <f>SUM(D2:D5)</f>
       </c>
     </row>
   </sheetData>

</xml_diff>